<commit_message>
fix test for DRY
</commit_message>
<xml_diff>
--- a/backend/data/cities.xlsx
+++ b/backend/data/cities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\projects\VolleyBolley\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCFB8052-B3A7-4730-8408-88892A2223BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4915197-C6B7-45AC-9E44-EE5AD86BE2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2568" windowWidth="20196" windowHeight="11112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -91,13 +91,19 @@
   </si>
   <si>
     <t>Paralimni</t>
+  </si>
+  <si>
+    <t>Deryneia</t>
+  </si>
+  <si>
+    <t>Polis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +120,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="204"/>
@@ -160,13 +173,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,146 +484,162 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>